<commit_message>
Further changes - mainly in Balve_3_plots
</commit_message>
<xml_diff>
--- a/analysis/Balve/raw_data/Balver_Höhle.xlsx
+++ b/analysis/Balve/raw_data/Balver_Höhle.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11576" uniqueCount="1863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11580" uniqueCount="1862">
   <si>
     <t>Balver_Höhle</t>
   </si>
@@ -5650,9 +5650,6 @@
   </si>
   <si>
     <t>0.048</t>
-  </si>
-  <si>
-    <t>1294.0</t>
   </si>
   <si>
     <t>perimeter basis.back</t>
@@ -6011,8 +6008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N167" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB190" sqref="AB190"/>
+    <sheetView tabSelected="1" topLeftCell="N313" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC313" sqref="AC313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6144,7 +6141,7 @@
         <v>1762</v>
       </c>
       <c r="AD1" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="AE1" t="s">
         <v>1763</v>
@@ -6387,8 +6384,8 @@
       <c r="AB3" t="s">
         <v>30</v>
       </c>
-      <c r="AC3" s="2" t="s">
-        <v>1859</v>
+      <c r="AC3" s="2">
+        <v>1.294</v>
       </c>
       <c r="AD3" t="s">
         <v>31</v>
@@ -9822,8 +9819,8 @@
       <c r="AB33" t="s">
         <v>268</v>
       </c>
-      <c r="AC33" s="2">
-        <v>0</v>
+      <c r="AC33" t="s">
+        <v>12</v>
       </c>
       <c r="AD33" t="s">
         <v>269</v>
@@ -9938,8 +9935,8 @@
       <c r="AB34" t="s">
         <v>279</v>
       </c>
-      <c r="AC34" s="2">
-        <v>0</v>
+      <c r="AC34" t="s">
+        <v>12</v>
       </c>
       <c r="AD34" t="s">
         <v>280</v>
@@ -10054,8 +10051,8 @@
       <c r="AB35" t="s">
         <v>288</v>
       </c>
-      <c r="AC35" s="2">
-        <v>0</v>
+      <c r="AC35" t="s">
+        <v>12</v>
       </c>
       <c r="AD35" t="s">
         <v>90</v>
@@ -10158,8 +10155,8 @@
       <c r="AB36" t="s">
         <v>296</v>
       </c>
-      <c r="AC36" s="2">
-        <v>0</v>
+      <c r="AC36" t="s">
+        <v>12</v>
       </c>
       <c r="AD36" t="s">
         <v>155</v>
@@ -27505,10 +27502,10 @@
         <v>39</v>
       </c>
       <c r="Z186" t="s">
+        <v>1860</v>
+      </c>
+      <c r="AA186" t="s">
         <v>1861</v>
-      </c>
-      <c r="AA186" t="s">
-        <v>1862</v>
       </c>
       <c r="AB186" t="s">
         <v>1107</v>
@@ -40397,8 +40394,8 @@
       <c r="AB313" t="s">
         <v>1592</v>
       </c>
-      <c r="AC313" s="2">
-        <v>0</v>
+      <c r="AC313" t="s">
+        <v>12</v>
       </c>
       <c r="AD313">
         <v>0</v>

</xml_diff>